<commit_message>
Added mesurements and accuracy
</commit_message>
<xml_diff>
--- a/1 mL Pipette/1 mL Pipette Mesurements.xlsx
+++ b/1 mL Pipette/1 mL Pipette Mesurements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Trial #</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>0.0193g</t>
+  </si>
+  <si>
+    <t>Percent Error</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -116,6 +119,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,6 +512,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>